<commit_message>
d326 data downloaded for preformat
</commit_message>
<xml_diff>
--- a/scripts/R-scripts/Biotic Interactions Snell/whatsgoingon.xlsx
+++ b/scripts/R-scripts/Biotic Interactions Snell/whatsgoingon.xlsx
@@ -98,7 +98,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -117,17 +117,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,81 +427,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BI - working on figures for poster
</commit_message>
<xml_diff>
--- a/scripts/R-scripts/Biotic Interactions Snell/whatsgoingon.xlsx
+++ b/scripts/R-scripts/Biotic Interactions Snell/whatsgoingon.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>green tailed towhee</t>
   </si>
@@ -62,14 +62,169 @@
     <t>foliage glean</t>
   </si>
   <si>
-    <t>?</t>
+    <t>ENV</t>
+  </si>
+  <si>
+    <t>COMP</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>AOU</t>
+  </si>
+  <si>
+    <t>DIET</t>
+  </si>
+  <si>
+    <t>FORAGE</t>
+  </si>
+  <si>
+    <t>white-crowned sparrow</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>SHARED</t>
+  </si>
+  <si>
+    <t>dense coniferous forest - diff distribution than the others</t>
+  </si>
+  <si>
+    <t>http://bna.birds.cornell.edu/bna/species/368/articles/introduction</t>
+  </si>
+  <si>
+    <t>W - lives in mountains, granivore, winters S</t>
+  </si>
+  <si>
+    <t>http://bna.birds.cornell.edu/bna/species/183/articles/introduction</t>
+  </si>
+  <si>
+    <t>NW - coastal scrub/chapparl, winters S</t>
+  </si>
+  <si>
+    <t>W - higher altitude, insectivore, winters S</t>
+  </si>
+  <si>
+    <t>http://bna.birds.cornell.edu/bna/species/280/articles/introduction</t>
+  </si>
+  <si>
+    <t>W - forest, winters S</t>
+  </si>
+  <si>
+    <t>http://bna.birds.cornell.edu/bna/species/240/articles/introduction</t>
+  </si>
+  <si>
+    <t>W - high elevations, coniferous forest, winters S</t>
+  </si>
+  <si>
+    <t>http://bna.birds.cornell.edu/bna/species/542/articles/introduction</t>
+  </si>
+  <si>
+    <t>middle - grassland/prairie, winters S</t>
+  </si>
+  <si>
+    <r>
+      <t>Editor’s Note: The Winter Wren discussed in this account (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>T. troglodytes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) has recently been split into 3 species, with </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>T. pacificus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (Pacific Wren) and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>T. hiemalis </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Winter Wren) the 2 North American species. See the 51st Supplement to the American Ornithologists’ Union </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Checklist of North American Birds</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and references therein, for details. Future revisions of this account will reflect these changes.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.000000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,13 +233,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Lucida Sans"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -97,6 +261,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -104,17 +280,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFCFD4D8"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFCFD4D8"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -132,21 +297,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="169" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,89 +612,275 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1">
+        <v>5900</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="E2" s="8">
+        <v>0.459475676</v>
+      </c>
+      <c r="F2" s="9">
+        <v>0.26140740000000001</v>
+      </c>
+      <c r="G2" s="9">
+        <v>-6.4261470000000001E-2</v>
+      </c>
+      <c r="H2" s="9">
+        <v>0.34337839999999997</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5540</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0.42912357699999998</v>
+      </c>
+      <c r="F3" s="9">
+        <v>3.8818819999999997E-2</v>
+      </c>
+      <c r="G3" s="9">
+        <v>3.1937989999999999E-2</v>
+      </c>
+      <c r="H3" s="9">
+        <v>0.5001196</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="1">
+        <v>6150</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E4" s="8">
+        <v>0.34002505799999999</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0.15196470000000001</v>
+      </c>
+      <c r="G4" s="9">
+        <v>4.63813E-2</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0.46162890000000001</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="6"/>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" s="5">
+        <v>5330</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="E5" s="8">
+        <v>0.26635562400000001</v>
+      </c>
+      <c r="F5" s="9">
+        <v>2.8207550000000001E-2</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0.24969359999999999</v>
+      </c>
+      <c r="H5" s="9">
+        <v>0.45574320000000001</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="1">
+        <v>5180</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="E6" s="9">
+        <v>0.18193701200000001</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0.36422739999999998</v>
+      </c>
+      <c r="G6" s="9">
+        <v>-5.4177400000000001E-2</v>
+      </c>
+      <c r="H6" s="9">
+        <v>0.50801300000000005</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="1">
+        <v>6050</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="E7" s="10">
+        <v>0.17318403499999999</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.40899380000000002</v>
+      </c>
+      <c r="G7" s="10">
+        <v>9.1302560000000005E-2</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0.32651960000000002</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>12</v>
+      <c r="B8" s="1">
+        <v>7222</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="10">
+        <v>2.8871272E-2</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.46037980000000001</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0.1207954</v>
+      </c>
+      <c r="H8" s="10">
+        <v>0.38995360000000001</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>